<commit_message>
Push outputs from CI/CD (2025-10-28 07:39:13)
</commit_message>
<xml_diff>
--- a/production/watch-dk-CHECKED/Manufacturing/Assembly/ZSWatch-Watch-DevKit-bom.xlsx
+++ b/production/watch-dk-CHECKED/Manufacturing/Assembly/ZSWatch-Watch-DevKit-bom.xlsx
@@ -257,7 +257,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>90665 Auf Lager</t>
+          <t>90565 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -307,7 +307,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>23556 Auf Lager</t>
+          <t>20026 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -357,7 +357,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>155619 Auf Lager</t>
+          <t>148627 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -406,7 +406,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>6946 Auf Lager</t>
+          <t>6436 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -423,7 +423,8 @@
   Qty  -  Unit€  -  Ext€
 ================
      1   €0.10      €0.10
-    10   €0.07      €0.67
+    10   €0.09      €0.86
+  5000   €0.08    €390.00
  10000   €0.04    €400.00
  20000   €0.03    €660.00</t>
         </r>
@@ -451,7 +452,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1710 Auf Lager</t>
+          <t>1375 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -501,7 +502,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>9392 Auf Lager</t>
+          <t>1132 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -518,11 +519,12 @@
   Qty  -  Unit€  -  Ext€
 ================
      1   €0.41      €0.41
-    10   €0.39      €3.89
-   100   €0.31     €30.70
-   500   €0.24    €121.50
-  2000   €0.19    €388.00
- 10000   €0.19  €1,880.00</t>
+    10   €0.41      €4.09
+   100   €0.31     €31.40
+   500   €0.26    €129.00
+  1000   €0.24    €243.00
+  2000   €0.20    €394.00
+ 10000   €0.19  €1,900.00</t>
         </r>
       </text>
     </comment>
@@ -548,7 +550,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>9392 Auf Lager</t>
+          <t>1132 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -565,11 +567,12 @@
   Qty  -  Unit€  -  Ext€
 ================
      1   €0.41      €0.41
-    10   €0.39      €3.89
-   100   €0.31     €30.70
-   500   €0.24    €121.50
-  2000   €0.19    €388.00
- 10000   €0.19  €1,880.00</t>
+    10   €0.41      €4.09
+   100   €0.31     €31.40
+   500   €0.26    €129.00
+  1000   €0.24    €243.00
+  2000   €0.20    €394.00
+ 10000   €0.19  €1,900.00</t>
         </r>
       </text>
     </comment>
@@ -595,7 +598,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>9392 Auf Lager</t>
+          <t>1132 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -612,11 +615,12 @@
   Qty  -  Unit€  -  Ext€
 ================
      1   €0.41      €0.41
-    10   €0.39      €3.89
-   100   €0.31     €30.70
-   500   €0.24    €121.50
-  2000   €0.19    €388.00
- 10000   €0.19  €1,880.00</t>
+    10   €0.41      €4.09
+   100   €0.31     €31.40
+   500   €0.26    €129.00
+  1000   €0.24    €243.00
+  2000   €0.20    €394.00
+ 10000   €0.19  €1,900.00</t>
         </r>
       </text>
     </comment>
@@ -642,7 +646,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>51553 Auf Lager</t>
+          <t>51503 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -691,7 +695,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>11498 Auf Lager</t>
+          <t>6083 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -742,7 +746,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>637 Auf Lager</t>
+          <t>This part is listed but is not stocked.</t>
         </r>
       </text>
     </comment>
@@ -843,7 +847,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>13507 Auf Lager</t>
+          <t>13501 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -959,7 +963,7 @@
           <t>Qty/Price Breaks (EUR):
   Qty  -  Unit€  -  Ext€
 ================
-  4800   €4.52 €21,696.00</t>
+  4800   €3.69 €17,712.00</t>
         </r>
       </text>
     </comment>
@@ -985,7 +989,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>19331 Auf Lager</t>
+          <t>13631 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1035,7 +1039,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>8288 Auf Lager</t>
+          <t>8263 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1133,7 +1137,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>187 Auf Lager</t>
+          <t>This part is listed but is not stocked.</t>
         </r>
       </text>
     </comment>
@@ -1224,7 +1228,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>86347 Auf Lager</t>
+          <t>80463 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1319,7 +1323,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>820 Auf Lager</t>
+          <t>788 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1363,7 +1367,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>25721 Auf Lager</t>
+          <t>25485 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1379,14 +1383,14 @@
           <t>Qty/Price Breaks (EUR):
   Qty  -  Unit€  -  Ext€
 ================
-     1   €1.46      €1.46
-    10   €1.20     €12.00
-    25   €1.10     €27.50
-    50   €1.03     €51.50
-   100   €0.97     €97.20
+     1   €1.63      €1.63
+    10   €1.28     €12.80
+    25   €1.16     €29.00
+    50   €1.08     €54.00
+   100   €1.01    €101.00
    250   €0.94    €234.25
-   500   €0.89    €443.00
-  1000   €0.86    €857.00
+   500   €0.89    €447.00
+  1000   €0.87    €869.00
   2500   €0.79  €1,975.00
   5700   €0.79  €4,503.00</t>
         </r>
@@ -1414,7 +1418,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>161980 Auf Lager</t>
+          <t>990 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1430,14 +1434,10 @@
           <t>Qty/Price Breaks (EUR):
   Qty  -  Unit€  -  Ext€
 ================
-     1   €0.29      €0.29
-    10   €0.16      €1.59
-   100   €0.10      €9.60
-   500   €0.08     €41.50
-  1000   €0.06     €64.00
-  2500   €0.06    €145.00
-  5000   €0.06    €275.00
- 10000   €0.06    €550.00</t>
+     1   €0.30      €0.30
+    10   €0.22      €2.18
+   100   €0.12     €12.40
+ 10000   €0.12  €1,240.00</t>
         </r>
       </text>
     </comment>
@@ -1463,7 +1463,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>31957 Auf Lager</t>
+          <t>14725 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1479,14 +1479,10 @@
           <t>Qty/Price Breaks (EUR):
   Qty  -  Unit€  -  Ext€
 ================
-     1   €0.27      €0.27
-    10   €0.16      €1.64
-   100   €0.10      €9.50
-   500   €0.09     €44.50
-  1000   €0.07     €69.00
-  2500   €0.07    €162.50
-  5000   €0.06    €315.00
- 10000   €0.06    €630.00</t>
+     1   €0.33      €0.33
+    10   €0.23      €2.30
+   100   €0.14     €13.80
+ 10000   €0.14  €1,380.00</t>
         </r>
       </text>
     </comment>
@@ -1512,7 +1508,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>86756 Auf Lager</t>
+          <t>78177 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1559,7 +1555,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>257603 Auf Lager</t>
+          <t>135728 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1575,12 +1571,12 @@
           <t>Qty/Price Breaks (EUR):
   Qty  -  Unit€  -  Ext€
 ================
-     1   €0.09      €0.09
-    10   €0.01      €0.08
-   100   €0.01      €0.50
-  1000   €0.00      €4.00
-  2500   €0.00      €7.50
- 10000   €0.00     €20.00</t>
+     1   €0.10      €0.10
+    10   €0.01      €0.11
+   100   €0.01      €0.60
+  1000   €0.01      €5.00
+  2500   €0.00     €10.00
+ 10000   €0.00     €30.00</t>
         </r>
       </text>
     </comment>
@@ -1606,7 +1602,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>76371 Auf Lager</t>
+          <t>31595 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1652,7 +1648,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>86756 Auf Lager</t>
+          <t>78177 Auf Lager</t>
         </r>
       </text>
     </comment>
@@ -1734,7 +1730,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="367">
   <si>
     <t>Row</t>
   </si>
@@ -2705,6 +2701,9 @@
     <t>262-BMP581</t>
   </si>
   <si>
+    <t>NonStk</t>
+  </si>
+  <si>
     <t>595-DRV2603RUNT</t>
   </si>
   <si>
@@ -2714,9 +2713,6 @@
     <t>511-LIS2MDLTR</t>
   </si>
   <si>
-    <t>NonStk</t>
-  </si>
-  <si>
     <t>95-25U51245GZ4I00T</t>
   </si>
   <si>
@@ -2786,7 +2782,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-16 10:51:35</t>
+    <t>2025-10-28 07:45:33</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>
@@ -5227,7 +5223,7 @@
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
-        <v>41.7474</v>
+        <v>42.1426</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -5242,11 +5238,11 @@
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H58)</f>
-        <v>41.7474</v>
+        <v>42.1426</v>
       </c>
       <c r="M4" s="16">
         <f>SUM(M10:M58)</f>
-        <v>41.7474</v>
+        <v>42.1426</v>
       </c>
       <c r="N4" s="17" t="str">
         <f>(COUNTA(M10:M58)&amp;" of "&amp;ROWS(M10:M58)&amp;" parts found")</f>
@@ -5355,26 +5351,26 @@
       </c>
       <c r="G10" s="22">
         <f>IF(MIN(K10)&lt;&gt;0,MIN(K10),"")</f>
-        <v>0.0325416</v>
+        <v>0.032591999999999996</v>
       </c>
       <c r="H10" s="23">
         <f>IF(AND(ISNUMBER(F10),ISNUMBER(G10)),F10*G10,"")</f>
-        <v>0.423</v>
+        <v>0.4237</v>
       </c>
       <c r="I10" s="21">
-        <v>90665</v>
+        <v>90565</v>
       </c>
       <c r="J10" s="21"/>
       <c r="K10" s="22">
         <f>IFERROR(IF(OR(J10&gt;=L10,F10&gt;=L10),USD_EUR*LOOKUP(IF(J10="",F10,J10),{0,1,10,100,500,1000,2500,5000,10000,50000},{0.0,0.095,0.028,0.016,0.012,0.01,0.009,0.008,0.007,0.007}),"MOQ="&amp;L10),"")</f>
-        <v>0.0325416</v>
+        <v>0.032591999999999996</v>
       </c>
       <c r="L10" s="21">
         <v>1</v>
       </c>
       <c r="M10" s="23">
         <f>IFERROR(IF(J10="",F10,J10)*K10,"")</f>
-        <v>0.423</v>
+        <v>0.4237</v>
       </c>
       <c r="N10" s="21" t="s">
         <v>314</v>
@@ -5402,26 +5398,26 @@
       </c>
       <c r="G11" s="22">
         <f>IF(MIN(K11)&lt;&gt;0,MIN(K11),"")</f>
-        <v>0.36957959999999995</v>
+        <v>0.370152</v>
       </c>
       <c r="H11" s="23">
         <f>IF(AND(ISNUMBER(F11),ISNUMBER(G11)),F11*G11,"")</f>
-        <v>0.3696</v>
+        <v>0.3702</v>
       </c>
       <c r="I11" s="21">
-        <v>23556</v>
+        <v>20026</v>
       </c>
       <c r="J11" s="21"/>
       <c r="K11" s="22">
         <f>IFERROR(IF(OR(J11&gt;=L11,F11&gt;=L11),USD_EUR*LOOKUP(IF(J11="",F11,J11),{0,1,10,100,500,1000,2500,5000,10000,20000},{0.0,0.318,0.206,0.129,0.104,0.095,0.089,0.088,0.075,0.071}),"MOQ="&amp;L11),"")</f>
-        <v>0.36957959999999995</v>
+        <v>0.370152</v>
       </c>
       <c r="L11" s="21">
         <v>1</v>
       </c>
       <c r="M11" s="23">
         <f>IFERROR(IF(J11="",F11,J11)*K11,"")</f>
-        <v>0.3696</v>
+        <v>0.3702</v>
       </c>
       <c r="N11" s="21" t="s">
         <v>315</v>
@@ -5449,26 +5445,26 @@
       </c>
       <c r="G12" s="22">
         <f>IF(MIN(K12)&lt;&gt;0,MIN(K12),"")</f>
-        <v>0.110409</v>
+        <v>0.11058</v>
       </c>
       <c r="H12" s="23">
         <f>IF(AND(ISNUMBER(F12),ISNUMBER(G12)),F12*G12,"")</f>
-        <v>0.3312</v>
+        <v>0.3317</v>
       </c>
       <c r="I12" s="21">
-        <v>155619</v>
+        <v>148627</v>
       </c>
       <c r="J12" s="21"/>
       <c r="K12" s="22">
         <f>IFERROR(IF(OR(J12&gt;=L12,F12&gt;=L12),USD_EUR*LOOKUP(IF(J12="",F12,J12),{0,1,10,100,500,1000,2500,5000,10000},{0.0,0.095,0.056,0.034,0.027,0.024,0.022,0.02,0.015}),"MOQ="&amp;L12),"")</f>
-        <v>0.110409</v>
+        <v>0.11058</v>
       </c>
       <c r="L12" s="21">
         <v>1</v>
       </c>
       <c r="M12" s="23">
         <f>IFERROR(IF(J12="",F12,J12)*K12,"")</f>
-        <v>0.3312</v>
+        <v>0.3317</v>
       </c>
       <c r="N12" s="21" t="s">
         <v>316</v>
@@ -5496,26 +5492,26 @@
       </c>
       <c r="G13" s="22">
         <f>IF(MIN(K13)&lt;&gt;0,MIN(K13),"")</f>
-        <v>0.11970659999999998</v>
+        <v>0.11989199999999998</v>
       </c>
       <c r="H13" s="23">
         <f>IF(AND(ISNUMBER(F13),ISNUMBER(G13)),F13*G13,"")</f>
-        <v>0.1197</v>
+        <v>0.1199</v>
       </c>
       <c r="I13" s="21">
-        <v>6946</v>
+        <v>6436</v>
       </c>
       <c r="J13" s="21"/>
       <c r="K13" s="22">
-        <f>IFERROR(IF(OR(J13&gt;=L13,F13&gt;=L13),USD_EUR*LOOKUP(IF(J13="",F13,J13),{0,1,10,10000,20000},{0.0,0.103,0.067,0.04,0.033}),"MOQ="&amp;L13),"")</f>
-        <v>0.11970659999999998</v>
+        <f>IFERROR(IF(OR(J13&gt;=L13,F13&gt;=L13),USD_EUR*LOOKUP(IF(J13="",F13,J13),{0,1,10,5000,10000,20000},{0.0,0.103,0.086,0.078,0.04,0.033}),"MOQ="&amp;L13),"")</f>
+        <v>0.11989199999999998</v>
       </c>
       <c r="L13" s="21">
         <v>1</v>
       </c>
       <c r="M13" s="23">
         <f>IFERROR(IF(J13="",F13,J13)*K13,"")</f>
-        <v>0.1197</v>
+        <v>0.1199</v>
       </c>
       <c r="N13" s="21" t="s">
         <v>317</v>
@@ -5572,26 +5568,26 @@
       </c>
       <c r="G15" s="22">
         <f>IF(MIN(K15)&lt;&gt;0,MIN(K15),"")</f>
-        <v>0.18943859999999998</v>
+        <v>0.18973199999999998</v>
       </c>
       <c r="H15" s="23">
         <f>IF(AND(ISNUMBER(F15),ISNUMBER(G15)),F15*G15,"")</f>
-        <v>0.5683</v>
+        <v>0.5692</v>
       </c>
       <c r="I15" s="21">
-        <v>1710</v>
+        <v>1375</v>
       </c>
       <c r="J15" s="21"/>
       <c r="K15" s="22">
         <f>IFERROR(IF(OR(J15&gt;=L15,F15&gt;=L15),USD_EUR*LOOKUP(IF(J15="",F15,J15),{0,1,10,100,500,1000,2000,4000,8000,24000},{0.0,0.163,0.108,0.056,0.045,0.04,0.036,0.027,0.025,0.024}),"MOQ="&amp;L15),"")</f>
-        <v>0.18943859999999998</v>
+        <v>0.18973199999999998</v>
       </c>
       <c r="L15" s="21">
         <v>1</v>
       </c>
       <c r="M15" s="23">
         <f>IFERROR(IF(J15="",F15,J15)*K15,"")</f>
-        <v>0.5683</v>
+        <v>0.5692</v>
       </c>
       <c r="N15" s="21" t="s">
         <v>318</v>
@@ -5619,26 +5615,26 @@
       </c>
       <c r="G16" s="22">
         <f>IF(MIN(K16)&lt;&gt;0,MIN(K16),"")</f>
-        <v>0.47998859999999993</v>
+        <v>0.48073199999999994</v>
       </c>
       <c r="H16" s="23">
         <f>IF(AND(ISNUMBER(F16),ISNUMBER(G16)),F16*G16,"")</f>
-        <v>0.48</v>
+        <v>0.4807</v>
       </c>
       <c r="I16" s="21">
-        <v>9392</v>
+        <v>1132</v>
       </c>
       <c r="J16" s="21"/>
       <c r="K16" s="22">
-        <f>IFERROR(IF(OR(J16&gt;=L16,F16&gt;=L16),USD_EUR*LOOKUP(IF(J16="",F16,J16),{0,1,10,100,500,2000,10000},{0.0,0.413,0.389,0.307,0.243,0.194,0.188}),"MOQ="&amp;L16),"")</f>
-        <v>0.47998859999999993</v>
+        <f>IFERROR(IF(OR(J16&gt;=L16,F16&gt;=L16),USD_EUR*LOOKUP(IF(J16="",F16,J16),{0,1,10,100,500,1000,2000,10000},{0.0,0.413,0.409,0.314,0.258,0.243,0.197,0.19}),"MOQ="&amp;L16),"")</f>
+        <v>0.48073199999999994</v>
       </c>
       <c r="L16" s="21">
         <v>1</v>
       </c>
       <c r="M16" s="23">
         <f>IFERROR(IF(J16="",F16,J16)*K16,"")</f>
-        <v>0.48</v>
+        <v>0.4807</v>
       </c>
       <c r="N16" s="21" t="s">
         <v>319</v>
@@ -5666,26 +5662,26 @@
       </c>
       <c r="G17" s="22">
         <f>IF(MIN(K17)&lt;&gt;0,MIN(K17),"")</f>
-        <v>0.47998859999999993</v>
+        <v>0.48073199999999994</v>
       </c>
       <c r="H17" s="23">
         <f>IF(AND(ISNUMBER(F17),ISNUMBER(G17)),F17*G17,"")</f>
-        <v>0.48</v>
+        <v>0.4807</v>
       </c>
       <c r="I17" s="21">
-        <v>9392</v>
+        <v>1132</v>
       </c>
       <c r="J17" s="21"/>
       <c r="K17" s="22">
-        <f>IFERROR(IF(OR(J17&gt;=L17,F17&gt;=L17),USD_EUR*LOOKUP(IF(J17="",F17,J17),{0,1,10,100,500,2000,10000},{0.0,0.413,0.389,0.307,0.243,0.194,0.188}),"MOQ="&amp;L17),"")</f>
-        <v>0.47998859999999993</v>
+        <f>IFERROR(IF(OR(J17&gt;=L17,F17&gt;=L17),USD_EUR*LOOKUP(IF(J17="",F17,J17),{0,1,10,100,500,1000,2000,10000},{0.0,0.413,0.409,0.314,0.258,0.243,0.197,0.19}),"MOQ="&amp;L17),"")</f>
+        <v>0.48073199999999994</v>
       </c>
       <c r="L17" s="21">
         <v>1</v>
       </c>
       <c r="M17" s="23">
         <f>IFERROR(IF(J17="",F17,J17)*K17,"")</f>
-        <v>0.48</v>
+        <v>0.4807</v>
       </c>
       <c r="N17" s="21" t="s">
         <v>319</v>
@@ -5713,26 +5709,26 @@
       </c>
       <c r="G18" s="22">
         <f>IF(MIN(K18)&lt;&gt;0,MIN(K18),"")</f>
-        <v>0.47998859999999993</v>
+        <v>0.48073199999999994</v>
       </c>
       <c r="H18" s="23">
         <f>IF(AND(ISNUMBER(F18),ISNUMBER(G18)),F18*G18,"")</f>
-        <v>0.48</v>
+        <v>0.4807</v>
       </c>
       <c r="I18" s="21">
-        <v>9392</v>
+        <v>1132</v>
       </c>
       <c r="J18" s="21"/>
       <c r="K18" s="22">
-        <f>IFERROR(IF(OR(J18&gt;=L18,F18&gt;=L18),USD_EUR*LOOKUP(IF(J18="",F18,J18),{0,1,10,100,500,2000,10000},{0.0,0.413,0.389,0.307,0.243,0.194,0.188}),"MOQ="&amp;L18),"")</f>
-        <v>0.47998859999999993</v>
+        <f>IFERROR(IF(OR(J18&gt;=L18,F18&gt;=L18),USD_EUR*LOOKUP(IF(J18="",F18,J18),{0,1,10,100,500,1000,2000,10000},{0.0,0.413,0.409,0.314,0.258,0.243,0.197,0.19}),"MOQ="&amp;L18),"")</f>
+        <v>0.48073199999999994</v>
       </c>
       <c r="L18" s="21">
         <v>1</v>
       </c>
       <c r="M18" s="23">
         <f>IFERROR(IF(J18="",F18,J18)*K18,"")</f>
-        <v>0.48</v>
+        <v>0.4807</v>
       </c>
       <c r="N18" s="21" t="s">
         <v>319</v>
@@ -5760,26 +5756,26 @@
       </c>
       <c r="G19" s="22">
         <f>IF(MIN(K19)&lt;&gt;0,MIN(K19),"")</f>
-        <v>0.9797345999999999</v>
+        <v>0.9812519999999999</v>
       </c>
       <c r="H19" s="23">
         <f>IF(AND(ISNUMBER(F19),ISNUMBER(G19)),F19*G19,"")</f>
-        <v>0.9797</v>
+        <v>0.9813</v>
       </c>
       <c r="I19" s="21">
-        <v>51553</v>
+        <v>51503</v>
       </c>
       <c r="J19" s="21"/>
       <c r="K19" s="22">
         <f>IFERROR(IF(OR(J19&gt;=L19,F19&gt;=L19),USD_EUR*LOOKUP(IF(J19="",F19,J19),{0,1,10,100,500,1000,2500,5000,10000},{0.0,0.843,0.712,0.681,0.618,0.595,0.567,0.538,0.519}),"MOQ="&amp;L19),"")</f>
-        <v>0.9797345999999999</v>
+        <v>0.9812519999999999</v>
       </c>
       <c r="L19" s="21">
         <v>1</v>
       </c>
       <c r="M19" s="23">
         <f>IFERROR(IF(J19="",F19,J19)*K19,"")</f>
-        <v>0.9797</v>
+        <v>0.9813</v>
       </c>
       <c r="N19" s="21" t="s">
         <v>320</v>
@@ -5807,26 +5803,26 @@
       </c>
       <c r="G20" s="22">
         <f>IF(MIN(K20)&lt;&gt;0,MIN(K20),"")</f>
-        <v>3.7422839999999997</v>
+        <v>3.74808</v>
       </c>
       <c r="H20" s="23">
         <f>IF(AND(ISNUMBER(F20),ISNUMBER(G20)),F20*G20,"")</f>
-        <v>3.7423</v>
+        <v>3.7481</v>
       </c>
       <c r="I20" s="21">
-        <v>11498</v>
+        <v>6083</v>
       </c>
       <c r="J20" s="21"/>
       <c r="K20" s="22">
         <f>IFERROR(IF(OR(J20&gt;=L20,F20&gt;=L20),USD_EUR*LOOKUP(IF(J20="",F20,J20),{0,1,5,10,25,50,100,500,1000,2500,5000},{0.0,3.22,2.87,2.75,2.61,2.5,2.41,2.22,2.18,2.0,2.0}),"MOQ="&amp;L20),"")</f>
-        <v>3.7422839999999997</v>
+        <v>3.74808</v>
       </c>
       <c r="L20" s="21">
         <v>1</v>
       </c>
       <c r="M20" s="23">
         <f>IFERROR(IF(J20="",F20,J20)*K20,"")</f>
-        <v>3.7423</v>
+        <v>3.7481</v>
       </c>
       <c r="N20" s="21" t="s">
         <v>321</v>
@@ -5854,26 +5850,26 @@
       </c>
       <c r="G21" s="22">
         <f>IF(MIN(K21)&lt;&gt;0,MIN(K21),"")</f>
-        <v>2.9752319999999997</v>
+        <v>2.97984</v>
       </c>
       <c r="H21" s="23">
         <f>IF(AND(ISNUMBER(F21),ISNUMBER(G21)),F21*G21,"")</f>
-        <v>2.9752</v>
-      </c>
-      <c r="I21" s="21">
-        <v>637</v>
+        <v>2.9798</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>323</v>
       </c>
       <c r="J21" s="21"/>
       <c r="K21" s="22">
         <f>IFERROR(IF(OR(J21&gt;=L21,F21&gt;=L21),USD_EUR*LOOKUP(IF(J21="",F21,J21),{0,1,5,10,50,100,500,1000,2000,5000,10000},{0.0,2.56,2.29,2.06,1.98,1.9,1.74,1.68,1.64,1.57,1.57}),"MOQ="&amp;L21),"")</f>
-        <v>2.9752319999999997</v>
+        <v>2.97984</v>
       </c>
       <c r="L21" s="21">
         <v>1</v>
       </c>
       <c r="M21" s="23">
         <f>IFERROR(IF(J21="",F21,J21)*K21,"")</f>
-        <v>2.9752</v>
+        <v>2.9798</v>
       </c>
       <c r="N21" s="21" t="s">
         <v>322</v>
@@ -5901,11 +5897,11 @@
       </c>
       <c r="G22" s="22">
         <f>IF(MIN(K22)&lt;&gt;0,MIN(K22),"")</f>
-        <v>1.6154579999999998</v>
+        <v>1.6179599999999998</v>
       </c>
       <c r="H22" s="23">
         <f>IF(AND(ISNUMBER(F22),ISNUMBER(G22)),F22*G22,"")</f>
-        <v>1.6155</v>
+        <v>1.618</v>
       </c>
       <c r="I22" s="21">
         <v>807</v>
@@ -5913,17 +5909,17 @@
       <c r="J22" s="21"/>
       <c r="K22" s="22">
         <f>IFERROR(IF(OR(J22&gt;=L22,F22&gt;=L22),USD_EUR*LOOKUP(IF(J22="",F22,J22),{0,1,10,25,100,250,500,1000,2500,5000},{0.0,1.39,1.02,0.929,0.826,0.777,0.732,0.706,0.696,0.667}),"MOQ="&amp;L22),"")</f>
-        <v>1.6154579999999998</v>
+        <v>1.6179599999999998</v>
       </c>
       <c r="L22" s="21">
         <v>1</v>
       </c>
       <c r="M22" s="23">
         <f>IFERROR(IF(J22="",F22,J22)*K22,"")</f>
-        <v>1.6155</v>
+        <v>1.618</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -5948,29 +5944,29 @@
       </c>
       <c r="G23" s="22">
         <f>IF(MIN(K23)&lt;&gt;0,MIN(K23),"")</f>
-        <v>1.1598756</v>
+        <v>1.1616719999999998</v>
       </c>
       <c r="H23" s="23">
         <f>IF(AND(ISNUMBER(F23),ISNUMBER(G23)),F23*G23,"")</f>
-        <v>1.1599</v>
+        <v>1.1617</v>
       </c>
       <c r="I23" s="21">
-        <v>13507</v>
+        <v>13501</v>
       </c>
       <c r="J23" s="21"/>
       <c r="K23" s="22">
         <f>IFERROR(IF(OR(J23&gt;=L23,F23&gt;=L23),USD_EUR*LOOKUP(IF(J23="",F23,J23),{0,1,10,25,100,250,500,1000,3000,6000},{0.0,0.998,0.447,0.394,0.334,0.303,0.286,0.264,0.238,0.234}),"MOQ="&amp;L23),"")</f>
-        <v>1.1598756</v>
+        <v>1.1616719999999998</v>
       </c>
       <c r="L23" s="21">
         <v>1</v>
       </c>
       <c r="M23" s="23">
         <f>IFERROR(IF(J23="",F23,J23)*K23,"")</f>
-        <v>1.1599</v>
+        <v>1.1617</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -5995,29 +5991,29 @@
       </c>
       <c r="G24" s="22">
         <f>IF(MIN(K24)&lt;&gt;0,MIN(K24),"")</f>
-        <v>2.138448</v>
+        <v>2.14176</v>
       </c>
       <c r="H24" s="23">
         <f>IF(AND(ISNUMBER(F24),ISNUMBER(G24)),F24*G24,"")</f>
-        <v>2.1384</v>
+        <v>2.1418</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="J24" s="21"/>
       <c r="K24" s="22">
         <f>IFERROR(IF(OR(J24&gt;=L24,F24&gt;=L24),USD_EUR*LOOKUP(IF(J24="",F24,J24),{0,1,5,10,50,100,500,1000,2000,10000},{0.0,1.84,1.63,1.47,1.41,1.35,1.24,1.2,1.18,1.18}),"MOQ="&amp;L24),"")</f>
-        <v>2.138448</v>
+        <v>2.14176</v>
       </c>
       <c r="L24" s="21">
         <v>1</v>
       </c>
       <c r="M24" s="23">
         <f>IFERROR(IF(J24="",F24,J24)*K24,"")</f>
-        <v>2.1384</v>
+        <v>2.1418</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -6049,11 +6045,11 @@
         <v/>
       </c>
       <c r="I25" s="24" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="J25" s="21"/>
       <c r="K25" s="22">
-        <f>IFERROR(IF(OR(J25&gt;=L25,F25&gt;=L25),USD_EUR*LOOKUP(IF(J25="",F25,J25),{0,1,4800},{0.0,4.52,4.52}),"MOQ="&amp;L25),"")</f>
+        <f>IFERROR(IF(OR(J25&gt;=L25,F25&gt;=L25),USD_EUR*LOOKUP(IF(J25="",F25,J25),{0,1,4800},{0.0,3.69,3.69}),"MOQ="&amp;L25),"")</f>
         <v/>
       </c>
       <c r="L25" s="21">
@@ -6089,26 +6085,26 @@
       </c>
       <c r="G26" s="22">
         <f>IF(MIN(K26)&lt;&gt;0,MIN(K26),"")</f>
-        <v>1.0297091999999999</v>
+        <v>1.031304</v>
       </c>
       <c r="H26" s="23">
         <f>IF(AND(ISNUMBER(F26),ISNUMBER(G26)),F26*G26,"")</f>
-        <v>1.0297</v>
+        <v>1.0313</v>
       </c>
       <c r="I26" s="21">
-        <v>19331</v>
+        <v>13631</v>
       </c>
       <c r="J26" s="21"/>
       <c r="K26" s="22">
         <f>IFERROR(IF(OR(J26&gt;=L26,F26&gt;=L26),USD_EUR*LOOKUP(IF(J26="",F26,J26),{0,1,10,25,100,250,500,1000,4000,8000},{0.0,0.886,0.638,0.576,0.508,0.476,0.451,0.441,0.373,0.371}),"MOQ="&amp;L26),"")</f>
-        <v>1.0297091999999999</v>
+        <v>1.031304</v>
       </c>
       <c r="L26" s="21">
         <v>1</v>
       </c>
       <c r="M26" s="23">
         <f>IFERROR(IF(J26="",F26,J26)*K26,"")</f>
-        <v>1.0297</v>
+        <v>1.0313</v>
       </c>
       <c r="N26" s="21" t="s">
         <v>328</v>
@@ -6136,26 +6132,26 @@
       </c>
       <c r="G27" s="22">
         <f>IF(MIN(K27)&lt;&gt;0,MIN(K27),"")</f>
-        <v>0.6601295999999999</v>
+        <v>0.6611519999999999</v>
       </c>
       <c r="H27" s="23">
         <f>IF(AND(ISNUMBER(F27),ISNUMBER(G27)),F27*G27,"")</f>
-        <v>0.6601</v>
+        <v>0.6612</v>
       </c>
       <c r="I27" s="21">
-        <v>8288</v>
+        <v>8263</v>
       </c>
       <c r="J27" s="21"/>
       <c r="K27" s="22">
         <f>IFERROR(IF(OR(J27&gt;=L27,F27&gt;=L27),USD_EUR*LOOKUP(IF(J27="",F27,J27),{0,1,10,25,100,250,500,1000,6000},{0.0,0.568,0.403,0.363,0.317,0.295,0.282,0.277,0.276}),"MOQ="&amp;L27),"")</f>
-        <v>0.6601295999999999</v>
+        <v>0.6611519999999999</v>
       </c>
       <c r="L27" s="21">
         <v>1</v>
       </c>
       <c r="M27" s="23">
         <f>IFERROR(IF(J27="",F27,J27)*K27,"")</f>
-        <v>0.6601</v>
+        <v>0.6612</v>
       </c>
       <c r="N27" s="21" t="s">
         <v>329</v>
@@ -6183,11 +6179,11 @@
       </c>
       <c r="G28" s="22">
         <f>IF(MIN(K28)&lt;&gt;0,MIN(K28),"")</f>
-        <v>2.09196</v>
+        <v>2.0951999999999997</v>
       </c>
       <c r="H28" s="23">
         <f>IF(AND(ISNUMBER(F28),ISNUMBER(G28)),F28*G28,"")</f>
-        <v>2.092</v>
+        <v>2.0952</v>
       </c>
       <c r="I28" s="21">
         <v>1667</v>
@@ -6195,14 +6191,14 @@
       <c r="J28" s="21"/>
       <c r="K28" s="22">
         <f>IFERROR(IF(OR(J28&gt;=L28,F28&gt;=L28),USD_EUR*LOOKUP(IF(J28="",F28,J28),{0,1,10,25,100,500,1000,4000,8000},{0.0,1.8,1.32,1.2,1.06,1.03,0.887,0.836,0.811}),"MOQ="&amp;L28),"")</f>
-        <v>2.09196</v>
+        <v>2.0951999999999997</v>
       </c>
       <c r="L28" s="21">
         <v>1</v>
       </c>
       <c r="M28" s="23">
         <f>IFERROR(IF(J28="",F28,J28)*K28,"")</f>
-        <v>2.092</v>
+        <v>2.0952</v>
       </c>
       <c r="N28" s="21" t="s">
         <v>330</v>
@@ -6230,26 +6226,26 @@
       </c>
       <c r="G29" s="22">
         <f>IF(MIN(K29)&lt;&gt;0,MIN(K29),"")</f>
-        <v>0.43931159999999997</v>
+        <v>0.439992</v>
       </c>
       <c r="H29" s="23">
         <f>IF(AND(ISNUMBER(F29),ISNUMBER(G29)),F29*G29,"")</f>
-        <v>0.4393</v>
-      </c>
-      <c r="I29" s="21">
-        <v>187</v>
+        <v>0.44</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>323</v>
       </c>
       <c r="J29" s="21"/>
       <c r="K29" s="22">
         <f>IFERROR(IF(OR(J29&gt;=L29,F29&gt;=L29),USD_EUR*LOOKUP(IF(J29="",F29,J29),{0,1,10,100,500,1000,3000},{0.0,0.378,0.256,0.174,0.136,0.121,0.087}),"MOQ="&amp;L29),"")</f>
-        <v>0.43931159999999997</v>
+        <v>0.439992</v>
       </c>
       <c r="L29" s="21">
         <v>1</v>
       </c>
       <c r="M29" s="23">
         <f>IFERROR(IF(J29="",F29,J29)*K29,"")</f>
-        <v>0.4393</v>
+        <v>0.44</v>
       </c>
       <c r="N29" s="21" t="s">
         <v>331</v>
@@ -6277,11 +6273,11 @@
       </c>
       <c r="G30" s="22">
         <f>IF(MIN(K30)&lt;&gt;0,MIN(K30),"")</f>
-        <v>4.1258099999999995</v>
+        <v>4.132199999999999</v>
       </c>
       <c r="H30" s="23">
         <f>IF(AND(ISNUMBER(F30),ISNUMBER(G30)),F30*G30,"")</f>
-        <v>4.1258</v>
+        <v>4.1322</v>
       </c>
       <c r="I30" s="21">
         <v>2343</v>
@@ -6289,14 +6285,14 @@
       <c r="J30" s="21"/>
       <c r="K30" s="22">
         <f>IFERROR(IF(OR(J30&gt;=L30,F30&gt;=L30),USD_EUR*LOOKUP(IF(J30="",F30,J30),{0,1,1000,1500},{0.0,3.55,2.78,2.78}),"MOQ="&amp;L30),"")</f>
-        <v>4.1258099999999995</v>
+        <v>4.132199999999999</v>
       </c>
       <c r="L30" s="21">
         <v>1</v>
       </c>
       <c r="M30" s="23">
         <f>IFERROR(IF(J30="",F30,J30)*K30,"")</f>
-        <v>4.1258</v>
+        <v>4.1322</v>
       </c>
       <c r="N30" s="21" t="s">
         <v>332</v>
@@ -6324,26 +6320,26 @@
       </c>
       <c r="G31" s="22">
         <f>IF(MIN(K31)&lt;&gt;0,MIN(K31),"")</f>
-        <v>0.3103074</v>
+        <v>0.310788</v>
       </c>
       <c r="H31" s="23">
         <f>IF(AND(ISNUMBER(F31),ISNUMBER(G31)),F31*G31,"")</f>
-        <v>3.4134</v>
+        <v>3.4187</v>
       </c>
       <c r="I31" s="21">
-        <v>86347</v>
+        <v>80463</v>
       </c>
       <c r="J31" s="21"/>
       <c r="K31" s="22">
         <f>IFERROR(IF(OR(J31&gt;=L31,F31&gt;=L31),USD_EUR*LOOKUP(IF(J31="",F31,J31),{0,1,50,100,500},{0.0,0.267,0.246,0.226,0.206}),"MOQ="&amp;L31),"")</f>
-        <v>0.3103074</v>
+        <v>0.310788</v>
       </c>
       <c r="L31" s="21">
         <v>1</v>
       </c>
       <c r="M31" s="23">
         <f>IFERROR(IF(J31="",F31,J31)*K31,"")</f>
-        <v>3.4134</v>
+        <v>3.4187</v>
       </c>
       <c r="N31" s="21" t="s">
         <v>333</v>
@@ -6371,11 +6367,11 @@
       </c>
       <c r="G32" s="22">
         <f>IF(MIN(K32)&lt;&gt;0,MIN(K32),"")</f>
-        <v>0.2998476</v>
+        <v>0.30031199999999997</v>
       </c>
       <c r="H32" s="23">
         <f>IF(AND(ISNUMBER(F32),ISNUMBER(G32)),F32*G32,"")</f>
-        <v>0.5997</v>
+        <v>0.6006</v>
       </c>
       <c r="I32" s="21">
         <v>4740</v>
@@ -6383,14 +6379,14 @@
       <c r="J32" s="21"/>
       <c r="K32" s="22">
         <f>IFERROR(IF(OR(J32&gt;=L32,F32&gt;=L32),USD_EUR*LOOKUP(IF(J32="",F32,J32),{0,1,10,25,100,250,1000,3000,6000,9000},{0.0,0.258,0.211,0.195,0.157,0.152,0.118,0.105,0.101,0.091}),"MOQ="&amp;L32),"")</f>
-        <v>0.2998476</v>
+        <v>0.30031199999999997</v>
       </c>
       <c r="L32" s="21">
         <v>1</v>
       </c>
       <c r="M32" s="23">
         <f>IFERROR(IF(J32="",F32,J32)*K32,"")</f>
-        <v>0.5997</v>
+        <v>0.6006</v>
       </c>
       <c r="N32" s="21" t="s">
         <v>334</v>
@@ -6418,26 +6414,26 @@
       </c>
       <c r="G33" s="22">
         <f>IF(MIN(K33)&lt;&gt;0,MIN(K33),"")</f>
-        <v>9.100026</v>
+        <v>9.11412</v>
       </c>
       <c r="H33" s="23">
         <f>IF(AND(ISNUMBER(F33),ISNUMBER(G33)),F33*G33,"")</f>
-        <v>9.1</v>
+        <v>9.1141</v>
       </c>
       <c r="I33" s="21">
-        <v>820</v>
+        <v>788</v>
       </c>
       <c r="J33" s="21"/>
       <c r="K33" s="22">
         <f>IFERROR(IF(OR(J33&gt;=L33,F33&gt;=L33),USD_EUR*LOOKUP(IF(J33="",F33,J33),{0,1,10,500},{0.0,7.83,7.67,7.67}),"MOQ="&amp;L33),"")</f>
-        <v>9.100026</v>
+        <v>9.11412</v>
       </c>
       <c r="L33" s="21">
         <v>1</v>
       </c>
       <c r="M33" s="23">
         <f>IFERROR(IF(J33="",F33,J33)*K33,"")</f>
-        <v>9.1</v>
+        <v>9.1141</v>
       </c>
       <c r="N33" s="21" t="s">
         <v>335</v>
@@ -6465,26 +6461,26 @@
       </c>
       <c r="G34" s="22">
         <f>IF(MIN(K34)&lt;&gt;0,MIN(K34),"")</f>
-        <v>1.6968119999999998</v>
+        <v>1.8973199999999997</v>
       </c>
       <c r="H34" s="23">
         <f>IF(AND(ISNUMBER(F34),ISNUMBER(G34)),F34*G34,"")</f>
-        <v>1.6968</v>
+        <v>1.8973</v>
       </c>
       <c r="I34" s="21">
-        <v>25721</v>
+        <v>25485</v>
       </c>
       <c r="J34" s="21"/>
       <c r="K34" s="22">
-        <f>IFERROR(IF(OR(J34&gt;=L34,F34&gt;=L34),USD_EUR*LOOKUP(IF(J34="",F34,J34),{0,1,10,25,50,100,250,500,1000,2500,5700},{0.0,1.46,1.2,1.1,1.03,0.972,0.937,0.886,0.857,0.79,0.79}),"MOQ="&amp;L34),"")</f>
-        <v>1.6968119999999998</v>
+        <f>IFERROR(IF(OR(J34&gt;=L34,F34&gt;=L34),USD_EUR*LOOKUP(IF(J34="",F34,J34),{0,1,10,25,50,100,250,500,1000,2500,5700},{0.0,1.63,1.28,1.16,1.08,1.01,0.937,0.894,0.869,0.79,0.79}),"MOQ="&amp;L34),"")</f>
+        <v>1.8973199999999997</v>
       </c>
       <c r="L34" s="21">
         <v>1</v>
       </c>
       <c r="M34" s="23">
         <f>IFERROR(IF(J34="",F34,J34)*K34,"")</f>
-        <v>1.6968</v>
+        <v>1.8973</v>
       </c>
       <c r="N34" s="21" t="s">
         <v>336</v>
@@ -6512,26 +6508,26 @@
       </c>
       <c r="G35" s="22">
         <f>IF(MIN(K35)&lt;&gt;0,MIN(K35),"")</f>
-        <v>0.33936239999999995</v>
+        <v>0.35036399999999995</v>
       </c>
       <c r="H35" s="23">
         <f>IF(AND(ISNUMBER(F35),ISNUMBER(G35)),F35*G35,"")</f>
-        <v>1.0181</v>
+        <v>1.0511</v>
       </c>
       <c r="I35" s="21">
-        <v>161980</v>
+        <v>990</v>
       </c>
       <c r="J35" s="21"/>
       <c r="K35" s="22">
-        <f>IFERROR(IF(OR(J35&gt;=L35,F35&gt;=L35),USD_EUR*LOOKUP(IF(J35="",F35,J35),{0,1,10,100,500,1000,2500,5000,10000},{0.0,0.292,0.159,0.096,0.083,0.064,0.058,0.055,0.055}),"MOQ="&amp;L35),"")</f>
-        <v>0.33936239999999995</v>
+        <f>IFERROR(IF(OR(J35&gt;=L35,F35&gt;=L35),USD_EUR*LOOKUP(IF(J35="",F35,J35),{0,1,10,100,10000},{0.0,0.301,0.218,0.124,0.124}),"MOQ="&amp;L35),"")</f>
+        <v>0.35036399999999995</v>
       </c>
       <c r="L35" s="21">
         <v>1</v>
       </c>
       <c r="M35" s="23">
         <f>IFERROR(IF(J35="",F35,J35)*K35,"")</f>
-        <v>1.0181</v>
+        <v>1.0511</v>
       </c>
       <c r="N35" s="21" t="s">
         <v>337</v>
@@ -6559,26 +6555,26 @@
       </c>
       <c r="G36" s="22">
         <f>IF(MIN(K36)&lt;&gt;0,MIN(K36),"")</f>
-        <v>0.3103074</v>
+        <v>0.38062799999999997</v>
       </c>
       <c r="H36" s="23">
         <f>IF(AND(ISNUMBER(F36),ISNUMBER(G36)),F36*G36,"")</f>
-        <v>0.3103</v>
+        <v>0.3806</v>
       </c>
       <c r="I36" s="21">
-        <v>31957</v>
+        <v>14725</v>
       </c>
       <c r="J36" s="21"/>
       <c r="K36" s="22">
-        <f>IFERROR(IF(OR(J36&gt;=L36,F36&gt;=L36),USD_EUR*LOOKUP(IF(J36="",F36,J36),{0,1,10,100,500,1000,2500,5000,10000},{0.0,0.267,0.164,0.095,0.089,0.069,0.065,0.063,0.063}),"MOQ="&amp;L36),"")</f>
-        <v>0.3103074</v>
+        <f>IFERROR(IF(OR(J36&gt;=L36,F36&gt;=L36),USD_EUR*LOOKUP(IF(J36="",F36,J36),{0,1,10,100,10000},{0.0,0.327,0.23,0.138,0.138}),"MOQ="&amp;L36),"")</f>
+        <v>0.38062799999999997</v>
       </c>
       <c r="L36" s="21">
         <v>1</v>
       </c>
       <c r="M36" s="23">
         <f>IFERROR(IF(J36="",F36,J36)*K36,"")</f>
-        <v>0.3103</v>
+        <v>0.3806</v>
       </c>
       <c r="N36" s="21" t="s">
         <v>338</v>
@@ -6606,26 +6602,26 @@
       </c>
       <c r="G37" s="22">
         <f>IF(MIN(K37)&lt;&gt;0,MIN(K37),"")</f>
-        <v>0.09994919999999999</v>
+        <v>0.10010399999999998</v>
       </c>
       <c r="H37" s="23">
         <f>IF(AND(ISNUMBER(F37),ISNUMBER(G37)),F37*G37,"")</f>
-        <v>0.8995</v>
+        <v>0.9009</v>
       </c>
       <c r="I37" s="21">
-        <v>86756</v>
+        <v>78177</v>
       </c>
       <c r="J37" s="21"/>
       <c r="K37" s="22">
         <f>IFERROR(IF(OR(J37&gt;=L37,F37&gt;=L37),USD_EUR*LOOKUP(IF(J37="",F37,J37),{0,1,10,100,1000,5000,25000},{0.0,0.086,0.008,0.005,0.004,0.003,0.002}),"MOQ="&amp;L37),"")</f>
-        <v>0.09994919999999999</v>
+        <v>0.10010399999999998</v>
       </c>
       <c r="L37" s="21">
         <v>1</v>
       </c>
       <c r="M37" s="23">
         <f>IFERROR(IF(J37="",F37,J37)*K37,"")</f>
-        <v>0.8995</v>
+        <v>0.9009</v>
       </c>
       <c r="N37" s="21" t="s">
         <v>339</v>
@@ -6653,26 +6649,26 @@
       </c>
       <c r="G38" s="22">
         <f>IF(MIN(K38)&lt;&gt;0,MIN(K38),"")</f>
-        <v>0.09994919999999999</v>
+        <v>0.11058</v>
       </c>
       <c r="H38" s="23">
         <f>IF(AND(ISNUMBER(F38),ISNUMBER(G38)),F38*G38,"")</f>
-        <v>0.2998</v>
+        <v>0.3317</v>
       </c>
       <c r="I38" s="21">
-        <v>257603</v>
+        <v>135728</v>
       </c>
       <c r="J38" s="21"/>
       <c r="K38" s="22">
-        <f>IFERROR(IF(OR(J38&gt;=L38,F38&gt;=L38),USD_EUR*LOOKUP(IF(J38="",F38,J38),{0,1,10,100,1000,2500,10000},{0.0,0.086,0.008,0.005,0.004,0.003,0.002}),"MOQ="&amp;L38),"")</f>
-        <v>0.09994919999999999</v>
+        <f>IFERROR(IF(OR(J38&gt;=L38,F38&gt;=L38),USD_EUR*LOOKUP(IF(J38="",F38,J38),{0,1,10,100,1000,2500,10000},{0.0,0.095,0.011,0.006,0.005,0.004,0.003}),"MOQ="&amp;L38),"")</f>
+        <v>0.11058</v>
       </c>
       <c r="L38" s="21">
         <v>1</v>
       </c>
       <c r="M38" s="23">
         <f>IFERROR(IF(J38="",F38,J38)*K38,"")</f>
-        <v>0.2998</v>
+        <v>0.3317</v>
       </c>
       <c r="N38" s="21" t="s">
         <v>340</v>
@@ -6758,26 +6754,26 @@
       </c>
       <c r="G41" s="22">
         <f>IF(MIN(K41)&lt;&gt;0,MIN(K41),"")</f>
-        <v>0.09994919999999999</v>
+        <v>0.10010399999999998</v>
       </c>
       <c r="H41" s="23">
         <f>IF(AND(ISNUMBER(F41),ISNUMBER(G41)),F41*G41,"")</f>
-        <v>0.0999</v>
+        <v>0.1001</v>
       </c>
       <c r="I41" s="21">
-        <v>76371</v>
+        <v>31595</v>
       </c>
       <c r="J41" s="21"/>
       <c r="K41" s="22">
         <f>IFERROR(IF(OR(J41&gt;=L41,F41&gt;=L41),USD_EUR*LOOKUP(IF(J41="",F41,J41),{0,1,10,100,1000,10000},{0.0,0.086,0.006,0.005,0.003,0.002}),"MOQ="&amp;L41),"")</f>
-        <v>0.09994919999999999</v>
+        <v>0.10010399999999998</v>
       </c>
       <c r="L41" s="21">
         <v>1</v>
       </c>
       <c r="M41" s="23">
         <f>IFERROR(IF(J41="",F41,J41)*K41,"")</f>
-        <v>0.0999</v>
+        <v>0.1001</v>
       </c>
       <c r="N41" s="21" t="s">
         <v>341</v>
@@ -6863,26 +6859,26 @@
       </c>
       <c r="G44" s="22">
         <f>IF(MIN(K44)&lt;&gt;0,MIN(K44),"")</f>
-        <v>0.09994919999999999</v>
+        <v>0.10010399999999998</v>
       </c>
       <c r="H44" s="23">
         <f>IF(AND(ISNUMBER(F44),ISNUMBER(G44)),F44*G44,"")</f>
-        <v>0.0999</v>
+        <v>0.1001</v>
       </c>
       <c r="I44" s="21">
-        <v>86756</v>
+        <v>78177</v>
       </c>
       <c r="J44" s="21"/>
       <c r="K44" s="22">
         <f>IFERROR(IF(OR(J44&gt;=L44,F44&gt;=L44),USD_EUR*LOOKUP(IF(J44="",F44,J44),{0,1,10,100,1000,5000,25000},{0.0,0.086,0.008,0.005,0.004,0.003,0.002}),"MOQ="&amp;L44),"")</f>
-        <v>0.09994919999999999</v>
+        <v>0.10010399999999998</v>
       </c>
       <c r="L44" s="21">
         <v>1</v>
       </c>
       <c r="M44" s="23">
         <f>IFERROR(IF(J44="",F44,J44)*K44,"")</f>
-        <v>0.0999</v>
+        <v>0.1001</v>
       </c>
       <c r="N44" s="21" t="s">
         <v>339</v>
@@ -7299,7 +7295,7 @@
         <v>345</v>
       </c>
       <c r="C60">
-        <v>1.1622</v>
+        <v>1.164</v>
       </c>
       <c r="G60" s="14" t="s">
         <v>343</v>

</xml_diff>